<commit_message>
With New SUP setup
</commit_message>
<xml_diff>
--- a/ANSWER-Veda Migration Log.xlsx
+++ b/ANSWER-Veda Migration Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIM-EL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AE29E5-8CA2-405B-8C5F-D6F5EA0037A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50439ACB-5583-4715-B6B6-539402CB3F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9465" yWindow="1335" windowWidth="19335" windowHeight="14265" xr2:uid="{010DEB55-B266-4EDB-AF61-05BEFBEEB6AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{010DEB55-B266-4EDB-AF61-05BEFBEEB6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Migration Log</t>
   </si>
@@ -89,29 +89,50 @@
     <t>Questions for Amit</t>
   </si>
   <si>
-    <t>FLO_EMISS?</t>
-  </si>
-  <si>
-    <t>COM_PROJ?</t>
-  </si>
-  <si>
-    <t>GAMS Engine credentials?</t>
-  </si>
-  <si>
-    <t>VO setup - linking to Git.</t>
-  </si>
-  <si>
-    <t>Is it possible to initiate the VO run from the command prompt?</t>
-  </si>
-  <si>
-    <t>Does the user get access to the GDX file when run is done?</t>
+    <t>Open questions</t>
+  </si>
+  <si>
+    <t>put fuel techs in sector workbooks or in SUP?</t>
+  </si>
+  <si>
+    <t>FLO_EMISS-&gt;COMEMI</t>
+  </si>
+  <si>
+    <t>In SUP so emission factors can be centrally controlled and reviewed</t>
+  </si>
+  <si>
+    <t>Outstanding issues</t>
+  </si>
+  <si>
+    <t>TCH_ELE</t>
+  </si>
+  <si>
+    <t>hydro flexibility</t>
+  </si>
+  <si>
+    <t>PWR_ENV</t>
+  </si>
+  <si>
+    <t>Questions for GAMS</t>
+  </si>
+  <si>
+    <t>how to setup GAMS Engine on UCT cluster, and how to launch runs from GAMS code/command prompt.</t>
+  </si>
+  <si>
+    <t>create a new sector for hgn production?</t>
+  </si>
+  <si>
+    <t>create a new sector for biomass production?</t>
+  </si>
+  <si>
+    <t>create a new workbook for LNG?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +160,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,10 +211,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -503,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69140962-8DE1-4028-A4EB-D25405C99763}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,72 +602,111 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="F33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>19</v>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>